<commit_message>
signature line and heading added to spreadsheet
</commit_message>
<xml_diff>
--- a/exports/SouthernLabs_WPE_Week_1.xlsx
+++ b/exports/SouthernLabs_WPE_Week_1.xlsx
@@ -17,13 +17,22 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00003366"/>
+      <sz val="16"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="12"/>
     </font>
     <font>
       <b val="1"/>
@@ -56,9 +65,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -424,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -432,195 +443,219 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="20" customWidth="1" min="5" max="5"/>
-    <col width="20" customWidth="1" min="6" max="6"/>
-    <col width="20" customWidth="1" min="7" max="7"/>
-    <col width="20" customWidth="1" min="8" max="8"/>
-    <col width="20" customWidth="1" min="9" max="9"/>
-    <col width="20" customWidth="1" min="10" max="10"/>
-    <col width="20" customWidth="1" min="11" max="11"/>
-    <col width="20" customWidth="1" min="12" max="12"/>
+    <col width="22" customWidth="1" min="1" max="1"/>
+    <col width="22" customWidth="1" min="2" max="2"/>
+    <col width="22" customWidth="1" min="3" max="3"/>
+    <col width="22" customWidth="1" min="4" max="4"/>
+    <col width="22" customWidth="1" min="5" max="5"/>
+    <col width="22" customWidth="1" min="6" max="6"/>
+    <col width="22" customWidth="1" min="7" max="7"/>
+    <col width="22" customWidth="1" min="8" max="8"/>
+    <col width="22" customWidth="1" min="9" max="9"/>
+    <col width="22" customWidth="1" min="10" max="10"/>
+    <col width="22" customWidth="1" min="11" max="11"/>
+    <col width="22" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>First Name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Middle Name</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Last Name</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>ID/Passport</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Email</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Phone</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Ethnicity</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Gender</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Course</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Week</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Time</t>
-        </is>
-      </c>
-    </row>
+    <row r="1"/>
     <row r="2">
-      <c r="A2" t="n">
-        <v>3</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Busi</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Portia</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Dladla</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>9106130205083</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>lindiwekhumalo833@gmail.com</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>0671114441</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Black</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>WPE</t>
-        </is>
-      </c>
-      <c r="K2" t="n">
-        <v>1</v>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>2026-02-10 17:24:10</t>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>Southern Labs Institute of Technology</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>Attendance Report: WPE - Week 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="4"/>
+    <row r="5"/>
+    <row r="6">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>First Name</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>Middle Name</t>
+        </is>
+      </c>
+      <c r="D6" s="3" t="inlineStr">
+        <is>
+          <t>Last Name</t>
+        </is>
+      </c>
+      <c r="E6" s="3" t="inlineStr">
+        <is>
+          <t>ID/Passport</t>
+        </is>
+      </c>
+      <c r="F6" s="3" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="G6" s="3" t="inlineStr">
+        <is>
+          <t>Phone</t>
+        </is>
+      </c>
+      <c r="H6" s="3" t="inlineStr">
+        <is>
+          <t>Ethnicity</t>
+        </is>
+      </c>
+      <c r="I6" s="3" t="inlineStr">
+        <is>
+          <t>Gender</t>
+        </is>
+      </c>
+      <c r="J6" s="3" t="inlineStr">
+        <is>
+          <t>Course</t>
+        </is>
+      </c>
+      <c r="K6" s="3" t="inlineStr">
+        <is>
+          <t>Week</t>
+        </is>
+      </c>
+      <c r="L6" s="3" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Busi</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Portia</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Dladla</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>9106130205083</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>lindiwekhumalo833@gmail.com</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>0671114441</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>WPE</t>
+        </is>
+      </c>
+      <c r="K7" t="n">
+        <v>1</v>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>2026-02-10 17:24:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
         <v>4</v>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B8" t="inlineStr">
         <is>
           <t>Zinhle</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>Mbali</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>Msweli</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>0008170030081</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>idahkhumalo291@gmail.com</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>0671114441</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>Black</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>Female</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="J8" t="inlineStr">
         <is>
           <t>WPE</t>
         </is>
       </c>
-      <c r="K3" t="n">
+      <c r="K8" t="n">
         <v>1</v>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="L8" t="inlineStr">
         <is>
           <t>2026-02-10 18:05:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>Facilitator Signature: ___________________________</t>
         </is>
       </c>
     </row>

</xml_diff>